<commit_message>
ARLR predictions using algo
</commit_message>
<xml_diff>
--- a/output_Harris_RNN_opt.xlsx
+++ b/output_Harris_RNN_opt.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alano\evaptransmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FF754243-CF1F-4FB2-ABF4-FD01DFB3F313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2933FF45-A488-4B2F-AC4D-3D9599911103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6855" yWindow="2370" windowWidth="21600" windowHeight="12210"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_Harris_RNN_opt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -876,11 +886,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27:S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +898,7 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -902,27 +912,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.107</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7.9500000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8.5199999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8.5099999999999995E-2</v>
       </c>
@@ -944,8 +954,17 @@
       <c r="L6">
         <v>8.8853000000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>8.6858000000000005E-2</v>
+      </c>
+      <c r="P6">
+        <v>8.9991000000000002E-2</v>
+      </c>
+      <c r="R6">
+        <v>9.0861999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4.9099999999999998E-2</v>
       </c>
@@ -967,8 +986,17 @@
       <c r="L7">
         <v>5.0293999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>5.3406000000000002E-2</v>
+      </c>
+      <c r="P7">
+        <v>4.7835999999999997E-2</v>
+      </c>
+      <c r="R7">
+        <v>4.7636999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.14099999999999999</v>
       </c>
@@ -990,8 +1018,17 @@
       <c r="L8">
         <v>0.12967300000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>0.13233900000000001</v>
+      </c>
+      <c r="P8">
+        <v>0.12690499999999999</v>
+      </c>
+      <c r="R8">
+        <v>0.12996099999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.11</v>
       </c>
@@ -1013,8 +1050,17 @@
       <c r="L9">
         <v>0.11247699999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0.10993700000000001</v>
+      </c>
+      <c r="P9">
+        <v>0.111815</v>
+      </c>
+      <c r="R9">
+        <v>0.115898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5.8099999999999999E-2</v>
       </c>
@@ -1036,8 +1082,17 @@
       <c r="L10">
         <v>7.2166999999999995E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>6.6725000000000007E-2</v>
+      </c>
+      <c r="P10">
+        <v>7.5671000000000002E-2</v>
+      </c>
+      <c r="R10">
+        <v>7.2316000000000005E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.20799999999999999</v>
       </c>
@@ -1059,8 +1114,17 @@
       <c r="L11">
         <v>0.109849</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0.119032</v>
+      </c>
+      <c r="P11">
+        <v>0.109262</v>
+      </c>
+      <c r="R11">
+        <v>0.10351299999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6.4799999999999996E-2</v>
       </c>
@@ -1082,8 +1146,17 @@
       <c r="L12">
         <v>6.6465999999999997E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>6.6083000000000003E-2</v>
+      </c>
+      <c r="P12">
+        <v>6.6811999999999996E-2</v>
+      </c>
+      <c r="R12">
+        <v>6.6756999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8.8700000000000001E-2</v>
       </c>
@@ -1105,8 +1178,17 @@
       <c r="L13">
         <v>7.4795E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>7.3587E-2</v>
+      </c>
+      <c r="P13">
+        <v>7.3041999999999996E-2</v>
+      </c>
+      <c r="R13">
+        <v>7.4964000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1.9199999999999998E-2</v>
       </c>
@@ -1128,8 +1210,17 @@
       <c r="L14">
         <v>9.9249999999999998E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>7.3379999999999999E-3</v>
+      </c>
+      <c r="P14">
+        <v>1.2050999999999999E-2</v>
+      </c>
+      <c r="R14">
+        <v>1.5443E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3.2500000000000001E-2</v>
       </c>
@@ -1151,8 +1242,17 @@
       <c r="L15">
         <v>4.3700000000000003E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>4.4155E-2</v>
+      </c>
+      <c r="P15">
+        <v>3.9912000000000003E-2</v>
+      </c>
+      <c r="R15">
+        <v>4.1798000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4.4299999999999999E-2</v>
       </c>
@@ -1174,8 +1274,17 @@
       <c r="L16">
         <v>4.5864000000000002E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>4.7042E-2</v>
+      </c>
+      <c r="P16">
+        <v>4.4471999999999998E-2</v>
+      </c>
+      <c r="R16">
+        <v>4.6376000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5.1400000000000001E-2</v>
       </c>
@@ -1197,8 +1306,17 @@
       <c r="L17">
         <v>4.6063E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>4.7725999999999998E-2</v>
+      </c>
+      <c r="P17">
+        <v>4.861E-2</v>
+      </c>
+      <c r="R17">
+        <v>4.4171000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5.62E-2</v>
       </c>
@@ -1220,8 +1338,17 @@
       <c r="L18">
         <v>5.9871000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>5.8909999999999997E-2</v>
+      </c>
+      <c r="P18">
+        <v>5.9959999999999999E-2</v>
+      </c>
+      <c r="R18">
+        <v>6.0597999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4.1700000000000001E-2</v>
       </c>
@@ -1243,8 +1370,17 @@
       <c r="L19">
         <v>4.1112999999999997E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>4.0124E-2</v>
+      </c>
+      <c r="P19">
+        <v>3.9469999999999998E-2</v>
+      </c>
+      <c r="R19">
+        <v>4.0069E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>5.1499999999999997E-2</v>
       </c>
@@ -1266,8 +1402,17 @@
       <c r="L20">
         <v>4.6830999999999998E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>5.0401000000000001E-2</v>
+      </c>
+      <c r="P20">
+        <v>4.5955999999999997E-2</v>
+      </c>
+      <c r="R20">
+        <v>4.7384999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.05</v>
       </c>
@@ -1289,8 +1434,17 @@
       <c r="L21">
         <v>4.6489999999999997E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>4.5982000000000002E-2</v>
+      </c>
+      <c r="P21">
+        <v>4.9167000000000002E-2</v>
+      </c>
+      <c r="R21">
+        <v>4.6158999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4.8399999999999999E-2</v>
       </c>
@@ -1312,8 +1466,17 @@
       <c r="L22">
         <v>5.3608000000000003E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>4.8342999999999997E-2</v>
+      </c>
+      <c r="P22">
+        <v>5.4510000000000003E-2</v>
+      </c>
+      <c r="R22">
+        <v>5.4073999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>5.28E-2</v>
       </c>
@@ -1335,8 +1498,17 @@
       <c r="L23">
         <v>9.2380000000000004E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>9.3285999999999994E-2</v>
+      </c>
+      <c r="P23">
+        <v>9.2574000000000004E-2</v>
+      </c>
+      <c r="R23">
+        <v>9.2100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2.63E-2</v>
       </c>
@@ -1358,8 +1530,17 @@
       <c r="L24">
         <v>9.8292000000000004E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>9.8269999999999996E-2</v>
+      </c>
+      <c r="P24">
+        <v>9.7570000000000004E-2</v>
+      </c>
+      <c r="R24">
+        <v>9.5496999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4.82E-2</v>
       </c>
@@ -1381,8 +1562,17 @@
       <c r="L25">
         <v>4.0348000000000002E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>4.0446999999999997E-2</v>
+      </c>
+      <c r="P25">
+        <v>4.1928E-2</v>
+      </c>
+      <c r="R25">
+        <v>4.1709000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6.7100000000000007E-2</v>
       </c>
@@ -1404,8 +1594,17 @@
       <c r="L26">
         <v>6.4499000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>6.1883000000000001E-2</v>
+      </c>
+      <c r="P26">
+        <v>6.6808999999999993E-2</v>
+      </c>
+      <c r="R26">
+        <v>6.5483E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>6.1899999999999997E-2</v>
       </c>
@@ -1451,8 +1650,29 @@
         <f>ABS(L27-$A27)/$A27</f>
         <v>0.92092084006462038</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>1.013E-2</v>
+      </c>
+      <c r="O27" s="2">
+        <f>ABS(N27-$A27)/$A27</f>
+        <v>0.83634894991922459</v>
+      </c>
+      <c r="P27">
+        <v>1.0944000000000001E-2</v>
+      </c>
+      <c r="Q27" s="2">
+        <f>ABS(P27-$A27)/$A27</f>
+        <v>0.82319870759289171</v>
+      </c>
+      <c r="R27">
+        <v>1.3062000000000001E-2</v>
+      </c>
+      <c r="S27" s="2">
+        <f>ABS(R27-$A27)/$A27</f>
+        <v>0.78898222940226159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4.1799999999999997E-2</v>
       </c>
@@ -1488,7 +1708,7 @@
         <v>4.0064000000000002E-2</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" ref="K28:M28" si="2">ABS(J28-$A28)/$A28</f>
+        <f t="shared" ref="K28:S28" si="2">ABS(J28-$A28)/$A28</f>
         <v>4.1531100478468773E-2</v>
       </c>
       <c r="L28">
@@ -1498,8 +1718,29 @@
         <f t="shared" si="2"/>
         <v>0.18784688995215307</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>4.0989999999999999E-2</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="2"/>
+        <v>1.937799043062197E-2</v>
+      </c>
+      <c r="P28">
+        <v>3.8517999999999997E-2</v>
+      </c>
+      <c r="Q28" s="2">
+        <f t="shared" si="2"/>
+        <v>7.8516746411483263E-2</v>
+      </c>
+      <c r="R28">
+        <v>3.3201000000000001E-2</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="2"/>
+        <v>0.20571770334928222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0.04</v>
       </c>
@@ -1535,7 +1776,7 @@
         <v>6.4326999999999995E-2</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" ref="K29:M29" si="4">ABS(J29-$A29)/$A29</f>
+        <f t="shared" ref="K29:S29" si="4">ABS(J29-$A29)/$A29</f>
         <v>0.6081749999999998</v>
       </c>
       <c r="L29">
@@ -1545,8 +1786,29 @@
         <f t="shared" si="4"/>
         <v>0.37829999999999997</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>3.1836000000000003E-2</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="4"/>
+        <v>0.20409999999999995</v>
+      </c>
+      <c r="P29">
+        <v>3.4331E-2</v>
+      </c>
+      <c r="Q29" s="2">
+        <f t="shared" si="4"/>
+        <v>0.14172500000000002</v>
+      </c>
+      <c r="R29">
+        <v>3.0513999999999999E-2</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="4"/>
+        <v>0.23715000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6.4799999999999996E-2</v>
       </c>
@@ -1582,7 +1844,7 @@
         <v>2.6051999999999999E-2</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" ref="K30:M30" si="6">ABS(J30-$A30)/$A30</f>
+        <f t="shared" ref="K30:S30" si="6">ABS(J30-$A30)/$A30</f>
         <v>0.59796296296296292</v>
       </c>
       <c r="L30">
@@ -1592,8 +1854,29 @@
         <f t="shared" si="6"/>
         <v>0.99827160493827161</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>8.5470000000000008E-3</v>
+      </c>
+      <c r="O30" s="2">
+        <f t="shared" si="6"/>
+        <v>0.86810185185185185</v>
+      </c>
+      <c r="P30">
+        <v>-7.9500000000000003E-4</v>
+      </c>
+      <c r="Q30" s="2">
+        <f t="shared" si="6"/>
+        <v>1.0122685185185185</v>
+      </c>
+      <c r="R30">
+        <v>3.1489999999999999E-3</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="6"/>
+        <v>0.95140432098765437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>2</v>
       </c>
@@ -1620,6 +1903,18 @@
       <c r="M31" s="2">
         <f>AVERAGE(M27:M30)</f>
         <v>0.62133483373876119</v>
+      </c>
+      <c r="O31" s="2">
+        <f>AVERAGE(O27:O30)</f>
+        <v>0.48198219805042464</v>
+      </c>
+      <c r="Q31" s="2">
+        <f>AVERAGE(Q27:Q30)</f>
+        <v>0.51392724313072335</v>
+      </c>
+      <c r="S31" s="2">
+        <f>AVERAGE(S27:S30)</f>
+        <v>0.54581356343479959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimized param for runRNN
</commit_message>
<xml_diff>
--- a/output_Harris_RNN_opt.xlsx
+++ b/output_Harris_RNN_opt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alano\evaptransmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2933FF45-A488-4B2F-AC4D-3D9599911103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC804E97-FB5E-421B-98D2-80C524932012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_Harris_RNN_opt" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>actual</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>10-50-1, 2e5</t>
+  </si>
+  <si>
+    <t>10-50-1, 3e5</t>
+  </si>
+  <si>
+    <t>10-200-1, 1e5</t>
   </si>
 </sst>
 </file>
@@ -887,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27:S31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +904,7 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,31 +914,28 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.107</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7.9500000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8.5199999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8.5099999999999995E-2</v>
       </c>
@@ -951,20 +954,8 @@
       <c r="J6">
         <v>9.5488000000000003E-2</v>
       </c>
-      <c r="L6">
-        <v>8.8853000000000001E-2</v>
-      </c>
-      <c r="N6">
-        <v>8.6858000000000005E-2</v>
-      </c>
-      <c r="P6">
-        <v>8.9991000000000002E-2</v>
-      </c>
-      <c r="R6">
-        <v>9.0861999999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4.9099999999999998E-2</v>
       </c>
@@ -983,20 +974,8 @@
       <c r="J7">
         <v>4.2653999999999997E-2</v>
       </c>
-      <c r="L7">
-        <v>5.0293999999999998E-2</v>
-      </c>
-      <c r="N7">
-        <v>5.3406000000000002E-2</v>
-      </c>
-      <c r="P7">
-        <v>4.7835999999999997E-2</v>
-      </c>
-      <c r="R7">
-        <v>4.7636999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.14099999999999999</v>
       </c>
@@ -1015,20 +994,8 @@
       <c r="J8">
         <v>0.11834500000000001</v>
       </c>
-      <c r="L8">
-        <v>0.12967300000000001</v>
-      </c>
-      <c r="N8">
-        <v>0.13233900000000001</v>
-      </c>
-      <c r="P8">
-        <v>0.12690499999999999</v>
-      </c>
-      <c r="R8">
-        <v>0.12996099999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.11</v>
       </c>
@@ -1047,20 +1014,8 @@
       <c r="J9">
         <v>0.12013799999999999</v>
       </c>
-      <c r="L9">
-        <v>0.11247699999999999</v>
-      </c>
-      <c r="N9">
-        <v>0.10993700000000001</v>
-      </c>
-      <c r="P9">
-        <v>0.111815</v>
-      </c>
-      <c r="R9">
-        <v>0.115898</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5.8099999999999999E-2</v>
       </c>
@@ -1079,20 +1034,8 @@
       <c r="J10">
         <v>8.3385000000000001E-2</v>
       </c>
-      <c r="L10">
-        <v>7.2166999999999995E-2</v>
-      </c>
-      <c r="N10">
-        <v>6.6725000000000007E-2</v>
-      </c>
-      <c r="P10">
-        <v>7.5671000000000002E-2</v>
-      </c>
-      <c r="R10">
-        <v>7.2316000000000005E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.20799999999999999</v>
       </c>
@@ -1111,20 +1054,8 @@
       <c r="J11">
         <v>9.0993000000000004E-2</v>
       </c>
-      <c r="L11">
-        <v>0.109849</v>
-      </c>
-      <c r="N11">
-        <v>0.119032</v>
-      </c>
-      <c r="P11">
-        <v>0.109262</v>
-      </c>
-      <c r="R11">
-        <v>0.10351299999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6.4799999999999996E-2</v>
       </c>
@@ -1143,20 +1074,8 @@
       <c r="J12">
         <v>6.6647999999999999E-2</v>
       </c>
-      <c r="L12">
-        <v>6.6465999999999997E-2</v>
-      </c>
-      <c r="N12">
-        <v>6.6083000000000003E-2</v>
-      </c>
-      <c r="P12">
-        <v>6.6811999999999996E-2</v>
-      </c>
-      <c r="R12">
-        <v>6.6756999999999997E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8.8700000000000001E-2</v>
       </c>
@@ -1175,20 +1094,8 @@
       <c r="J13">
         <v>7.2123999999999994E-2</v>
       </c>
-      <c r="L13">
-        <v>7.4795E-2</v>
-      </c>
-      <c r="N13">
-        <v>7.3587E-2</v>
-      </c>
-      <c r="P13">
-        <v>7.3041999999999996E-2</v>
-      </c>
-      <c r="R13">
-        <v>7.4964000000000003E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1.9199999999999998E-2</v>
       </c>
@@ -1207,20 +1114,8 @@
       <c r="J14">
         <v>2.6085000000000001E-2</v>
       </c>
-      <c r="L14">
-        <v>9.9249999999999998E-3</v>
-      </c>
-      <c r="N14">
-        <v>7.3379999999999999E-3</v>
-      </c>
-      <c r="P14">
-        <v>1.2050999999999999E-2</v>
-      </c>
-      <c r="R14">
-        <v>1.5443E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3.2500000000000001E-2</v>
       </c>
@@ -1239,20 +1134,8 @@
       <c r="J15">
         <v>3.7762999999999998E-2</v>
       </c>
-      <c r="L15">
-        <v>4.3700000000000003E-2</v>
-      </c>
-      <c r="N15">
-        <v>4.4155E-2</v>
-      </c>
-      <c r="P15">
-        <v>3.9912000000000003E-2</v>
-      </c>
-      <c r="R15">
-        <v>4.1798000000000002E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4.4299999999999999E-2</v>
       </c>
@@ -1271,20 +1154,8 @@
       <c r="J16">
         <v>4.5421999999999997E-2</v>
       </c>
-      <c r="L16">
-        <v>4.5864000000000002E-2</v>
-      </c>
-      <c r="N16">
-        <v>4.7042E-2</v>
-      </c>
-      <c r="P16">
-        <v>4.4471999999999998E-2</v>
-      </c>
-      <c r="R16">
-        <v>4.6376000000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5.1400000000000001E-2</v>
       </c>
@@ -1303,20 +1174,8 @@
       <c r="J17">
         <v>4.3071999999999999E-2</v>
       </c>
-      <c r="L17">
-        <v>4.6063E-2</v>
-      </c>
-      <c r="N17">
-        <v>4.7725999999999998E-2</v>
-      </c>
-      <c r="P17">
-        <v>4.861E-2</v>
-      </c>
-      <c r="R17">
-        <v>4.4171000000000002E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5.62E-2</v>
       </c>
@@ -1335,20 +1194,8 @@
       <c r="J18">
         <v>5.9475E-2</v>
       </c>
-      <c r="L18">
-        <v>5.9871000000000001E-2</v>
-      </c>
-      <c r="N18">
-        <v>5.8909999999999997E-2</v>
-      </c>
-      <c r="P18">
-        <v>5.9959999999999999E-2</v>
-      </c>
-      <c r="R18">
-        <v>6.0597999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4.1700000000000001E-2</v>
       </c>
@@ -1367,20 +1214,8 @@
       <c r="J19">
         <v>4.3588000000000002E-2</v>
       </c>
-      <c r="L19">
-        <v>4.1112999999999997E-2</v>
-      </c>
-      <c r="N19">
-        <v>4.0124E-2</v>
-      </c>
-      <c r="P19">
-        <v>3.9469999999999998E-2</v>
-      </c>
-      <c r="R19">
-        <v>4.0069E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>5.1499999999999997E-2</v>
       </c>
@@ -1399,20 +1234,8 @@
       <c r="J20">
         <v>3.7859999999999998E-2</v>
       </c>
-      <c r="L20">
-        <v>4.6830999999999998E-2</v>
-      </c>
-      <c r="N20">
-        <v>5.0401000000000001E-2</v>
-      </c>
-      <c r="P20">
-        <v>4.5955999999999997E-2</v>
-      </c>
-      <c r="R20">
-        <v>4.7384999999999997E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.05</v>
       </c>
@@ -1431,20 +1254,8 @@
       <c r="J21">
         <v>5.5382000000000001E-2</v>
       </c>
-      <c r="L21">
-        <v>4.6489999999999997E-2</v>
-      </c>
-      <c r="N21">
-        <v>4.5982000000000002E-2</v>
-      </c>
-      <c r="P21">
-        <v>4.9167000000000002E-2</v>
-      </c>
-      <c r="R21">
-        <v>4.6158999999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4.8399999999999999E-2</v>
       </c>
@@ -1463,20 +1274,8 @@
       <c r="J22">
         <v>5.9133999999999999E-2</v>
       </c>
-      <c r="L22">
-        <v>5.3608000000000003E-2</v>
-      </c>
-      <c r="N22">
-        <v>4.8342999999999997E-2</v>
-      </c>
-      <c r="P22">
-        <v>5.4510000000000003E-2</v>
-      </c>
-      <c r="R22">
-        <v>5.4073999999999997E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>5.28E-2</v>
       </c>
@@ -1495,20 +1294,8 @@
       <c r="J23">
         <v>9.6278000000000002E-2</v>
       </c>
-      <c r="L23">
-        <v>9.2380000000000004E-2</v>
-      </c>
-      <c r="N23">
-        <v>9.3285999999999994E-2</v>
-      </c>
-      <c r="P23">
-        <v>9.2574000000000004E-2</v>
-      </c>
-      <c r="R23">
-        <v>9.2100000000000001E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2.63E-2</v>
       </c>
@@ -1527,20 +1314,8 @@
       <c r="J24">
         <v>8.5030999999999995E-2</v>
       </c>
-      <c r="L24">
-        <v>9.8292000000000004E-2</v>
-      </c>
-      <c r="N24">
-        <v>9.8269999999999996E-2</v>
-      </c>
-      <c r="P24">
-        <v>9.7570000000000004E-2</v>
-      </c>
-      <c r="R24">
-        <v>9.5496999999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4.82E-2</v>
       </c>
@@ -1559,20 +1334,8 @@
       <c r="J25">
         <v>4.5677000000000002E-2</v>
       </c>
-      <c r="L25">
-        <v>4.0348000000000002E-2</v>
-      </c>
-      <c r="N25">
-        <v>4.0446999999999997E-2</v>
-      </c>
-      <c r="P25">
-        <v>4.1928E-2</v>
-      </c>
-      <c r="R25">
-        <v>4.1709000000000003E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6.7100000000000007E-2</v>
       </c>
@@ -1591,20 +1354,8 @@
       <c r="J26">
         <v>7.0139999999999994E-2</v>
       </c>
-      <c r="L26">
-        <v>6.4499000000000001E-2</v>
-      </c>
-      <c r="N26">
-        <v>6.1883000000000001E-2</v>
-      </c>
-      <c r="P26">
-        <v>6.6808999999999993E-2</v>
-      </c>
-      <c r="R26">
-        <v>6.5483E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>6.1899999999999997E-2</v>
       </c>
@@ -1643,36 +1394,8 @@
         <f>ABS(J27-$A27)/$A27</f>
         <v>0.40699515347334414</v>
       </c>
-      <c r="L27">
-        <v>4.895E-3</v>
-      </c>
-      <c r="M27" s="2">
-        <f>ABS(L27-$A27)/$A27</f>
-        <v>0.92092084006462038</v>
-      </c>
-      <c r="N27">
-        <v>1.013E-2</v>
-      </c>
-      <c r="O27" s="2">
-        <f>ABS(N27-$A27)/$A27</f>
-        <v>0.83634894991922459</v>
-      </c>
-      <c r="P27">
-        <v>1.0944000000000001E-2</v>
-      </c>
-      <c r="Q27" s="2">
-        <f>ABS(P27-$A27)/$A27</f>
-        <v>0.82319870759289171</v>
-      </c>
-      <c r="R27">
-        <v>1.3062000000000001E-2</v>
-      </c>
-      <c r="S27" s="2">
-        <f>ABS(R27-$A27)/$A27</f>
-        <v>0.78898222940226159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4.1799999999999997E-2</v>
       </c>
@@ -1708,39 +1431,11 @@
         <v>4.0064000000000002E-2</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" ref="K28:S28" si="2">ABS(J28-$A28)/$A28</f>
+        <f t="shared" ref="K28" si="2">ABS(J28-$A28)/$A28</f>
         <v>4.1531100478468773E-2</v>
       </c>
-      <c r="L28">
-        <v>3.3947999999999999E-2</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="2"/>
-        <v>0.18784688995215307</v>
-      </c>
-      <c r="N28">
-        <v>4.0989999999999999E-2</v>
-      </c>
-      <c r="O28" s="2">
-        <f t="shared" si="2"/>
-        <v>1.937799043062197E-2</v>
-      </c>
-      <c r="P28">
-        <v>3.8517999999999997E-2</v>
-      </c>
-      <c r="Q28" s="2">
-        <f t="shared" si="2"/>
-        <v>7.8516746411483263E-2</v>
-      </c>
-      <c r="R28">
-        <v>3.3201000000000001E-2</v>
-      </c>
-      <c r="S28" s="2">
-        <f t="shared" si="2"/>
-        <v>0.20571770334928222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0.04</v>
       </c>
@@ -1776,39 +1471,11 @@
         <v>6.4326999999999995E-2</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" ref="K29:S29" si="4">ABS(J29-$A29)/$A29</f>
+        <f t="shared" ref="K29" si="4">ABS(J29-$A29)/$A29</f>
         <v>0.6081749999999998</v>
       </c>
-      <c r="L29">
-        <v>2.4868000000000001E-2</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="4"/>
-        <v>0.37829999999999997</v>
-      </c>
-      <c r="N29">
-        <v>3.1836000000000003E-2</v>
-      </c>
-      <c r="O29" s="2">
-        <f t="shared" si="4"/>
-        <v>0.20409999999999995</v>
-      </c>
-      <c r="P29">
-        <v>3.4331E-2</v>
-      </c>
-      <c r="Q29" s="2">
-        <f t="shared" si="4"/>
-        <v>0.14172500000000002</v>
-      </c>
-      <c r="R29">
-        <v>3.0513999999999999E-2</v>
-      </c>
-      <c r="S29" s="2">
-        <f t="shared" si="4"/>
-        <v>0.23715000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6.4799999999999996E-2</v>
       </c>
@@ -1844,39 +1511,11 @@
         <v>2.6051999999999999E-2</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" ref="K30:S30" si="6">ABS(J30-$A30)/$A30</f>
+        <f t="shared" ref="K30" si="6">ABS(J30-$A30)/$A30</f>
         <v>0.59796296296296292</v>
       </c>
-      <c r="L30">
-        <v>1.12E-4</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="6"/>
-        <v>0.99827160493827161</v>
-      </c>
-      <c r="N30">
-        <v>8.5470000000000008E-3</v>
-      </c>
-      <c r="O30" s="2">
-        <f t="shared" si="6"/>
-        <v>0.86810185185185185</v>
-      </c>
-      <c r="P30">
-        <v>-7.9500000000000003E-4</v>
-      </c>
-      <c r="Q30" s="2">
-        <f t="shared" si="6"/>
-        <v>1.0122685185185185</v>
-      </c>
-      <c r="R30">
-        <v>3.1489999999999999E-3</v>
-      </c>
-      <c r="S30" s="2">
-        <f t="shared" si="6"/>
-        <v>0.95140432098765437</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>2</v>
       </c>
@@ -1900,21 +1539,1323 @@
         <f>AVERAGE(K27:K30)</f>
         <v>0.41366605422869396</v>
       </c>
-      <c r="M31" s="2">
-        <f>AVERAGE(M27:M30)</f>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>8.8853000000000001E-2</v>
+      </c>
+      <c r="D34">
+        <v>8.6858000000000005E-2</v>
+      </c>
+      <c r="F34">
+        <v>8.9991000000000002E-2</v>
+      </c>
+      <c r="H34">
+        <v>9.0861999999999998E-2</v>
+      </c>
+      <c r="J34">
+        <v>8.9119000000000004E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>5.0293999999999998E-2</v>
+      </c>
+      <c r="D35">
+        <v>5.3406000000000002E-2</v>
+      </c>
+      <c r="F35">
+        <v>4.7835999999999997E-2</v>
+      </c>
+      <c r="H35">
+        <v>4.7636999999999999E-2</v>
+      </c>
+      <c r="J35">
+        <v>5.0737999999999998E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0.12967300000000001</v>
+      </c>
+      <c r="D36">
+        <v>0.13233900000000001</v>
+      </c>
+      <c r="F36">
+        <v>0.12690499999999999</v>
+      </c>
+      <c r="H36">
+        <v>0.12996099999999999</v>
+      </c>
+      <c r="J36">
+        <v>0.12973699999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>0.11247699999999999</v>
+      </c>
+      <c r="D37">
+        <v>0.10993700000000001</v>
+      </c>
+      <c r="F37">
+        <v>0.111815</v>
+      </c>
+      <c r="H37">
+        <v>0.115898</v>
+      </c>
+      <c r="J37">
+        <v>0.111911</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>7.2166999999999995E-2</v>
+      </c>
+      <c r="D38">
+        <v>6.6725000000000007E-2</v>
+      </c>
+      <c r="F38">
+        <v>7.5671000000000002E-2</v>
+      </c>
+      <c r="H38">
+        <v>7.2316000000000005E-2</v>
+      </c>
+      <c r="J38">
+        <v>7.2055999999999995E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0.109849</v>
+      </c>
+      <c r="D39">
+        <v>0.119032</v>
+      </c>
+      <c r="F39">
+        <v>0.109262</v>
+      </c>
+      <c r="H39">
+        <v>0.10351299999999999</v>
+      </c>
+      <c r="J39">
+        <v>0.11111</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>6.6465999999999997E-2</v>
+      </c>
+      <c r="D40">
+        <v>6.6083000000000003E-2</v>
+      </c>
+      <c r="F40">
+        <v>6.6811999999999996E-2</v>
+      </c>
+      <c r="H40">
+        <v>6.6756999999999997E-2</v>
+      </c>
+      <c r="J40">
+        <v>6.5881999999999996E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>7.4795E-2</v>
+      </c>
+      <c r="D41">
+        <v>7.3587E-2</v>
+      </c>
+      <c r="F41">
+        <v>7.3041999999999996E-2</v>
+      </c>
+      <c r="H41">
+        <v>7.4964000000000003E-2</v>
+      </c>
+      <c r="J41">
+        <v>7.2871000000000005E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>9.9249999999999998E-3</v>
+      </c>
+      <c r="D42">
+        <v>7.3379999999999999E-3</v>
+      </c>
+      <c r="F42">
+        <v>1.2050999999999999E-2</v>
+      </c>
+      <c r="H42">
+        <v>1.5443E-2</v>
+      </c>
+      <c r="J42">
+        <v>1.1707E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="D43">
+        <v>4.4155E-2</v>
+      </c>
+      <c r="F43">
+        <v>3.9912000000000003E-2</v>
+      </c>
+      <c r="H43">
+        <v>4.1798000000000002E-2</v>
+      </c>
+      <c r="J43">
+        <v>4.3060000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>4.5864000000000002E-2</v>
+      </c>
+      <c r="D44">
+        <v>4.7042E-2</v>
+      </c>
+      <c r="F44">
+        <v>4.4471999999999998E-2</v>
+      </c>
+      <c r="H44">
+        <v>4.6376000000000001E-2</v>
+      </c>
+      <c r="J44">
+        <v>4.5859999999999998E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>4.6063E-2</v>
+      </c>
+      <c r="D45">
+        <v>4.7725999999999998E-2</v>
+      </c>
+      <c r="F45">
+        <v>4.861E-2</v>
+      </c>
+      <c r="H45">
+        <v>4.4171000000000002E-2</v>
+      </c>
+      <c r="J45">
+        <v>4.7008000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>5.9871000000000001E-2</v>
+      </c>
+      <c r="D46">
+        <v>5.8909999999999997E-2</v>
+      </c>
+      <c r="F46">
+        <v>5.9959999999999999E-2</v>
+      </c>
+      <c r="H46">
+        <v>6.0597999999999999E-2</v>
+      </c>
+      <c r="J46">
+        <v>6.0714999999999998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>4.1112999999999997E-2</v>
+      </c>
+      <c r="D47">
+        <v>4.0124E-2</v>
+      </c>
+      <c r="F47">
+        <v>3.9469999999999998E-2</v>
+      </c>
+      <c r="H47">
+        <v>4.0069E-2</v>
+      </c>
+      <c r="J47">
+        <v>3.8913000000000003E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>4.6830999999999998E-2</v>
+      </c>
+      <c r="D48">
+        <v>5.0401000000000001E-2</v>
+      </c>
+      <c r="F48">
+        <v>4.5955999999999997E-2</v>
+      </c>
+      <c r="H48">
+        <v>4.7384999999999997E-2</v>
+      </c>
+      <c r="J48">
+        <v>4.8578999999999997E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>4.6489999999999997E-2</v>
+      </c>
+      <c r="D49">
+        <v>4.5982000000000002E-2</v>
+      </c>
+      <c r="F49">
+        <v>4.9167000000000002E-2</v>
+      </c>
+      <c r="H49">
+        <v>4.6158999999999999E-2</v>
+      </c>
+      <c r="J49">
+        <v>4.6505999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>5.3608000000000003E-2</v>
+      </c>
+      <c r="D50">
+        <v>4.8342999999999997E-2</v>
+      </c>
+      <c r="F50">
+        <v>5.4510000000000003E-2</v>
+      </c>
+      <c r="H50">
+        <v>5.4073999999999997E-2</v>
+      </c>
+      <c r="J50">
+        <v>5.1973999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>9.2380000000000004E-2</v>
+      </c>
+      <c r="D51">
+        <v>9.3285999999999994E-2</v>
+      </c>
+      <c r="F51">
+        <v>9.2574000000000004E-2</v>
+      </c>
+      <c r="H51">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="J51">
+        <v>9.3150999999999998E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>9.8292000000000004E-2</v>
+      </c>
+      <c r="D52">
+        <v>9.8269999999999996E-2</v>
+      </c>
+      <c r="F52">
+        <v>9.7570000000000004E-2</v>
+      </c>
+      <c r="H52">
+        <v>9.5496999999999999E-2</v>
+      </c>
+      <c r="J52">
+        <v>9.8221000000000003E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>4.0348000000000002E-2</v>
+      </c>
+      <c r="D53">
+        <v>4.0446999999999997E-2</v>
+      </c>
+      <c r="F53">
+        <v>4.1928E-2</v>
+      </c>
+      <c r="H53">
+        <v>4.1709000000000003E-2</v>
+      </c>
+      <c r="J53">
+        <v>3.9884999999999997E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>6.4499000000000001E-2</v>
+      </c>
+      <c r="D54">
+        <v>6.1883000000000001E-2</v>
+      </c>
+      <c r="F54">
+        <v>6.6808999999999993E-2</v>
+      </c>
+      <c r="H54">
+        <v>6.5483E-2</v>
+      </c>
+      <c r="J54">
+        <v>6.4380999999999994E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>4.895E-3</v>
+      </c>
+      <c r="C55" s="2">
+        <f>ABS(B55-$A27)/$A27</f>
+        <v>0.92092084006462038</v>
+      </c>
+      <c r="D55">
+        <v>1.013E-2</v>
+      </c>
+      <c r="E55" s="2">
+        <f>ABS(D55-$A27)/$A27</f>
+        <v>0.83634894991922459</v>
+      </c>
+      <c r="F55">
+        <v>1.0944000000000001E-2</v>
+      </c>
+      <c r="G55" s="2">
+        <f>ABS(F55-$A27)/$A27</f>
+        <v>0.82319870759289171</v>
+      </c>
+      <c r="H55">
+        <v>1.3062000000000001E-2</v>
+      </c>
+      <c r="I55" s="2">
+        <f>ABS(H55-$A27)/$A27</f>
+        <v>0.78898222940226159</v>
+      </c>
+      <c r="J55">
+        <v>7.339E-3</v>
+      </c>
+      <c r="K55" s="2">
+        <f>ABS(J55-$A27)/$A27</f>
+        <v>0.88143780290791607</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>3.3947999999999999E-2</v>
+      </c>
+      <c r="C56" s="2">
+        <f>ABS(B56-$A28)/$A28</f>
+        <v>0.18784688995215307</v>
+      </c>
+      <c r="D56">
+        <v>4.0989999999999999E-2</v>
+      </c>
+      <c r="E56" s="2">
+        <f>ABS(D56-$A28)/$A28</f>
+        <v>1.937799043062197E-2</v>
+      </c>
+      <c r="F56">
+        <v>3.8517999999999997E-2</v>
+      </c>
+      <c r="G56" s="2">
+        <f>ABS(F56-$A28)/$A28</f>
+        <v>7.8516746411483263E-2</v>
+      </c>
+      <c r="H56">
+        <v>3.3201000000000001E-2</v>
+      </c>
+      <c r="I56" s="2">
+        <f>ABS(H56-$A28)/$A28</f>
+        <v>0.20571770334928222</v>
+      </c>
+      <c r="J56">
+        <v>3.7347999999999999E-2</v>
+      </c>
+      <c r="K56" s="2">
+        <f>ABS(J56-$A28)/$A28</f>
+        <v>0.10650717703349277</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>2.4868000000000001E-2</v>
+      </c>
+      <c r="C57" s="2">
+        <f>ABS(B57-$A29)/$A29</f>
+        <v>0.37829999999999997</v>
+      </c>
+      <c r="D57">
+        <v>3.1836000000000003E-2</v>
+      </c>
+      <c r="E57" s="2">
+        <f>ABS(D57-$A29)/$A29</f>
+        <v>0.20409999999999995</v>
+      </c>
+      <c r="F57">
+        <v>3.4331E-2</v>
+      </c>
+      <c r="G57" s="2">
+        <f>ABS(F57-$A29)/$A29</f>
+        <v>0.14172500000000002</v>
+      </c>
+      <c r="H57">
+        <v>3.0513999999999999E-2</v>
+      </c>
+      <c r="I57" s="2">
+        <f>ABS(H57-$A29)/$A29</f>
+        <v>0.23715000000000003</v>
+      </c>
+      <c r="J57">
+        <v>3.2432000000000002E-2</v>
+      </c>
+      <c r="K57" s="2">
+        <f>ABS(J57-$A29)/$A29</f>
+        <v>0.18919999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>1.12E-4</v>
+      </c>
+      <c r="C58" s="2">
+        <f>ABS(B58-$A30)/$A30</f>
+        <v>0.99827160493827161</v>
+      </c>
+      <c r="D58">
+        <v>8.5470000000000008E-3</v>
+      </c>
+      <c r="E58" s="2">
+        <f>ABS(D58-$A30)/$A30</f>
+        <v>0.86810185185185185</v>
+      </c>
+      <c r="F58">
+        <v>-7.9500000000000003E-4</v>
+      </c>
+      <c r="G58" s="2">
+        <f>ABS(F58-$A30)/$A30</f>
+        <v>1.0122685185185185</v>
+      </c>
+      <c r="H58">
+        <v>3.1489999999999999E-3</v>
+      </c>
+      <c r="I58" s="2">
+        <f>ABS(H58-$A30)/$A30</f>
+        <v>0.95140432098765437</v>
+      </c>
+      <c r="J58">
+        <v>1.176E-3</v>
+      </c>
+      <c r="K58" s="2">
+        <f>ABS(J58-$A30)/$A30</f>
+        <v>0.98185185185185186</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="2">
+        <f>AVERAGE(C55:C58)</f>
         <v>0.62133483373876119</v>
       </c>
-      <c r="O31" s="2">
-        <f>AVERAGE(O27:O30)</f>
+      <c r="E59" s="2">
+        <f>AVERAGE(E55:E58)</f>
         <v>0.48198219805042464</v>
       </c>
-      <c r="Q31" s="2">
-        <f>AVERAGE(Q27:Q30)</f>
+      <c r="G59" s="2">
+        <f>AVERAGE(G55:G58)</f>
         <v>0.51392724313072335</v>
       </c>
-      <c r="S31" s="2">
-        <f>AVERAGE(S27:S30)</f>
+      <c r="I59" s="2">
+        <f>AVERAGE(I55:I58)</f>
         <v>0.54581356343479959</v>
+      </c>
+      <c r="K59" s="2">
+        <f>AVERAGE(K55:K58)</f>
+        <v>0.53974920794831516</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>8.5625999999999994E-2</v>
+      </c>
+      <c r="D62">
+        <v>8.5486999999999994E-2</v>
+      </c>
+      <c r="F62">
+        <v>8.6737999999999996E-2</v>
+      </c>
+      <c r="H62">
+        <v>8.6581000000000005E-2</v>
+      </c>
+      <c r="J62">
+        <v>8.6341000000000001E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>5.4158999999999999E-2</v>
+      </c>
+      <c r="D63">
+        <v>5.4921999999999999E-2</v>
+      </c>
+      <c r="F63">
+        <v>4.6198999999999997E-2</v>
+      </c>
+      <c r="H63">
+        <v>5.3925000000000001E-2</v>
+      </c>
+      <c r="J63">
+        <v>5.2510000000000001E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>0.13299900000000001</v>
+      </c>
+      <c r="D64">
+        <v>0.13527</v>
+      </c>
+      <c r="F64">
+        <v>0.13411699999999999</v>
+      </c>
+      <c r="H64">
+        <v>0.133469</v>
+      </c>
+      <c r="J64">
+        <v>0.13406499999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>0.108641</v>
+      </c>
+      <c r="D65">
+        <v>0.108113</v>
+      </c>
+      <c r="F65">
+        <v>0.109919</v>
+      </c>
+      <c r="H65">
+        <v>0.110281</v>
+      </c>
+      <c r="J65">
+        <v>0.10917499999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>6.0621000000000001E-2</v>
+      </c>
+      <c r="D66">
+        <v>5.3623999999999998E-2</v>
+      </c>
+      <c r="F66">
+        <v>5.9378E-2</v>
+      </c>
+      <c r="H66">
+        <v>6.028E-2</v>
+      </c>
+      <c r="J66">
+        <v>5.7521000000000003E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0.13163800000000001</v>
+      </c>
+      <c r="D67">
+        <v>0.14697299999999999</v>
+      </c>
+      <c r="F67">
+        <v>0.145978</v>
+      </c>
+      <c r="H67">
+        <v>0.12829499999999999</v>
+      </c>
+      <c r="J67">
+        <v>0.139678</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>6.6403000000000004E-2</v>
+      </c>
+      <c r="D68">
+        <v>6.4137E-2</v>
+      </c>
+      <c r="F68">
+        <v>7.2672E-2</v>
+      </c>
+      <c r="H68">
+        <v>6.6146999999999997E-2</v>
+      </c>
+      <c r="J68">
+        <v>6.5838999999999995E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>7.6478000000000004E-2</v>
+      </c>
+      <c r="D69">
+        <v>7.5457999999999997E-2</v>
+      </c>
+      <c r="F69">
+        <v>7.3335999999999998E-2</v>
+      </c>
+      <c r="H69">
+        <v>7.6763999999999999E-2</v>
+      </c>
+      <c r="J69">
+        <v>7.4741000000000002E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>2.1159999999999998E-3</v>
+      </c>
+      <c r="D70">
+        <v>5.7340000000000004E-3</v>
+      </c>
+      <c r="F70">
+        <v>-1.24E-3</v>
+      </c>
+      <c r="H70">
+        <v>4.5250000000000004E-3</v>
+      </c>
+      <c r="J70">
+        <v>4.3940000000000003E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>4.6690000000000002E-2</v>
+      </c>
+      <c r="D71">
+        <v>4.4222999999999998E-2</v>
+      </c>
+      <c r="F71">
+        <v>3.8418000000000001E-2</v>
+      </c>
+      <c r="H71">
+        <v>4.7941999999999999E-2</v>
+      </c>
+      <c r="J71">
+        <v>4.4027999999999998E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>4.3504000000000001E-2</v>
+      </c>
+      <c r="D72">
+        <v>4.4117999999999997E-2</v>
+      </c>
+      <c r="F72">
+        <v>4.6693999999999999E-2</v>
+      </c>
+      <c r="H72">
+        <v>4.2422000000000001E-2</v>
+      </c>
+      <c r="J72">
+        <v>4.4327999999999999E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>5.1493999999999998E-2</v>
+      </c>
+      <c r="D73">
+        <v>5.0955E-2</v>
+      </c>
+      <c r="F73">
+        <v>5.015E-2</v>
+      </c>
+      <c r="H73">
+        <v>5.0470000000000001E-2</v>
+      </c>
+      <c r="J73">
+        <v>5.1843E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>5.6274999999999999E-2</v>
+      </c>
+      <c r="D74">
+        <v>5.9514999999999998E-2</v>
+      </c>
+      <c r="F74">
+        <v>5.4425000000000001E-2</v>
+      </c>
+      <c r="H74">
+        <v>5.7603000000000001E-2</v>
+      </c>
+      <c r="J74">
+        <v>5.6937000000000001E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>4.2651000000000001E-2</v>
+      </c>
+      <c r="D75">
+        <v>4.0675999999999997E-2</v>
+      </c>
+      <c r="F75">
+        <v>4.5323000000000002E-2</v>
+      </c>
+      <c r="H75">
+        <v>4.1751000000000003E-2</v>
+      </c>
+      <c r="J75">
+        <v>4.2349999999999999E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>4.8857999999999999E-2</v>
+      </c>
+      <c r="D76">
+        <v>4.8556000000000002E-2</v>
+      </c>
+      <c r="F76">
+        <v>4.6147000000000001E-2</v>
+      </c>
+      <c r="H76">
+        <v>4.9283E-2</v>
+      </c>
+      <c r="J76">
+        <v>4.7951000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>4.8750000000000002E-2</v>
+      </c>
+      <c r="D77">
+        <v>5.1369999999999999E-2</v>
+      </c>
+      <c r="F77">
+        <v>5.4543000000000001E-2</v>
+      </c>
+      <c r="H77">
+        <v>4.7597E-2</v>
+      </c>
+      <c r="J77">
+        <v>5.0791000000000003E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>4.6519999999999999E-2</v>
+      </c>
+      <c r="D78">
+        <v>3.9716000000000001E-2</v>
+      </c>
+      <c r="F78">
+        <v>5.4601999999999998E-2</v>
+      </c>
+      <c r="H78">
+        <v>4.6741999999999999E-2</v>
+      </c>
+      <c r="J78">
+        <v>4.5428999999999997E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>9.1537999999999994E-2</v>
+      </c>
+      <c r="D79">
+        <v>9.2894000000000004E-2</v>
+      </c>
+      <c r="F79">
+        <v>7.6198000000000002E-2</v>
+      </c>
+      <c r="H79">
+        <v>9.1214000000000003E-2</v>
+      </c>
+      <c r="J79">
+        <v>8.9510999999999993E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>9.5154000000000002E-2</v>
+      </c>
+      <c r="D80">
+        <v>8.8723999999999997E-2</v>
+      </c>
+      <c r="F80">
+        <v>8.2729999999999998E-2</v>
+      </c>
+      <c r="H80">
+        <v>9.6216999999999997E-2</v>
+      </c>
+      <c r="J80">
+        <v>9.1819999999999999E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>4.0653000000000002E-2</v>
+      </c>
+      <c r="D81">
+        <v>4.4632999999999999E-2</v>
+      </c>
+      <c r="F81">
+        <v>4.8125000000000001E-2</v>
+      </c>
+      <c r="H81">
+        <v>3.9532999999999999E-2</v>
+      </c>
+      <c r="J81">
+        <v>4.2937000000000003E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>6.1468000000000002E-2</v>
+      </c>
+      <c r="D82">
+        <v>5.7475999999999999E-2</v>
+      </c>
+      <c r="F82">
+        <v>6.9579000000000002E-2</v>
+      </c>
+      <c r="H82">
+        <v>6.2246000000000003E-2</v>
+      </c>
+      <c r="J82">
+        <v>6.0789000000000003E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>-3.826E-3</v>
+      </c>
+      <c r="C83" s="2">
+        <f>ABS(B83-$A27)/$A27</f>
+        <v>1.0618093699515347</v>
+      </c>
+      <c r="D83">
+        <v>1.2161999999999999E-2</v>
+      </c>
+      <c r="E83" s="2">
+        <f>ABS(D83-$A27)/$A27</f>
+        <v>0.80352180936995155</v>
+      </c>
+      <c r="F83">
+        <v>-2.7743E-2</v>
+      </c>
+      <c r="G83" s="2">
+        <f>ABS(F83-$A27)/$A27</f>
+        <v>1.4481906300484653</v>
+      </c>
+      <c r="H83">
+        <v>-2.8860000000000001E-3</v>
+      </c>
+      <c r="I83" s="2">
+        <f>ABS(H83-$A27)/$A27</f>
+        <v>1.0466235864297253</v>
+      </c>
+      <c r="J83">
+        <v>4.1159999999999999E-3</v>
+      </c>
+      <c r="K83" s="2">
+        <f>ABS(J83-$A27)/$A27</f>
+        <v>0.93350565428109855</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>3.4991000000000001E-2</v>
+      </c>
+      <c r="C84" s="2">
+        <f>ABS(B84-$A28)/$A28</f>
+        <v>0.16289473684210518</v>
+      </c>
+      <c r="D84">
+        <v>4.4875999999999999E-2</v>
+      </c>
+      <c r="E84" s="2">
+        <f>ABS(D84-$A28)/$A28</f>
+        <v>7.358851674641155E-2</v>
+      </c>
+      <c r="F84">
+        <v>5.6982999999999999E-2</v>
+      </c>
+      <c r="G84" s="2">
+        <f>ABS(F84-$A28)/$A28</f>
+        <v>0.3632296650717704</v>
+      </c>
+      <c r="H84">
+        <v>3.2521000000000001E-2</v>
+      </c>
+      <c r="I84" s="2">
+        <f>ABS(H84-$A28)/$A28</f>
+        <v>0.22198564593301426</v>
+      </c>
+      <c r="J84">
+        <v>4.4127E-2</v>
+      </c>
+      <c r="K84" s="2">
+        <f>ABS(J84-$A28)/$A28</f>
+        <v>5.5669856459330209E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>-2.0439999999999998E-3</v>
+      </c>
+      <c r="C85" s="2">
+        <f>ABS(B85-$A29)/$A29</f>
+        <v>1.0510999999999999</v>
+      </c>
+      <c r="D85">
+        <v>2.0749E-2</v>
+      </c>
+      <c r="E85" s="2">
+        <f>ABS(D85-$A29)/$A29</f>
+        <v>0.48127500000000001</v>
+      </c>
+      <c r="F85">
+        <v>5.6389999999999999E-3</v>
+      </c>
+      <c r="G85" s="2">
+        <f>ABS(F85-$A29)/$A29</f>
+        <v>0.85902500000000004</v>
+      </c>
+      <c r="H85">
+        <v>-7.76E-4</v>
+      </c>
+      <c r="I85" s="2">
+        <f>ABS(H85-$A29)/$A29</f>
+        <v>1.0193999999999999</v>
+      </c>
+      <c r="J85">
+        <v>9.0349999999999996E-3</v>
+      </c>
+      <c r="K85" s="2">
+        <f>ABS(J85-$A29)/$A29</f>
+        <v>0.77412499999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>6.8849999999999996E-3</v>
+      </c>
+      <c r="C86" s="2">
+        <f>ABS(B86-$A30)/$A30</f>
+        <v>0.89374999999999993</v>
+      </c>
+      <c r="D86">
+        <v>2.0376999999999999E-2</v>
+      </c>
+      <c r="E86" s="2">
+        <f>ABS(D86-$A30)/$A30</f>
+        <v>0.68554012345679016</v>
+      </c>
+      <c r="F86">
+        <v>-4.1071000000000003E-2</v>
+      </c>
+      <c r="G86" s="2">
+        <f>ABS(F86-$A30)/$A30</f>
+        <v>1.6338117283950617</v>
+      </c>
+      <c r="H86">
+        <v>4.8079999999999998E-3</v>
+      </c>
+      <c r="I86" s="2">
+        <f>ABS(H86-$A30)/$A30</f>
+        <v>0.92580246913580244</v>
+      </c>
+      <c r="J86">
+        <v>1.6480000000000002E-2</v>
+      </c>
+      <c r="K86" s="2">
+        <f>ABS(J86-$A30)/$A30</f>
+        <v>0.74567901234567902</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C87" s="2">
+        <f>AVERAGE(C83:C86)</f>
+        <v>0.79238852669840987</v>
+      </c>
+      <c r="E87" s="2">
+        <f>AVERAGE(E83:E86)</f>
+        <v>0.51098136239328829</v>
+      </c>
+      <c r="G87" s="2">
+        <f>AVERAGE(G83:G86)</f>
+        <v>1.0760642558788245</v>
+      </c>
+      <c r="I87" s="2">
+        <f>AVERAGE(I83:I86)</f>
+        <v>0.80345292537463542</v>
+      </c>
+      <c r="K87" s="2">
+        <f>AVERAGE(K83:K86)</f>
+        <v>0.62724488077152696</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>9.6092999999999998E-2</v>
+      </c>
+      <c r="D91">
+        <v>9.6159999999999995E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>4.3135E-2</v>
+      </c>
+      <c r="D92">
+        <v>4.3306999999999998E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>0.118907</v>
+      </c>
+      <c r="D93">
+        <v>0.118491</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0.120557</v>
+      </c>
+      <c r="D94">
+        <v>0.120142</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>8.3157999999999996E-2</v>
+      </c>
+      <c r="D95">
+        <v>8.3538000000000001E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>9.0384000000000006E-2</v>
+      </c>
+      <c r="D96">
+        <v>9.0428999999999995E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>6.6292000000000004E-2</v>
+      </c>
+      <c r="D97">
+        <v>6.6979999999999998E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>7.1541999999999994E-2</v>
+      </c>
+      <c r="D98">
+        <v>7.0963999999999999E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>2.6974999999999999E-2</v>
+      </c>
+      <c r="D99">
+        <v>2.6776000000000001E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>3.8592000000000001E-2</v>
+      </c>
+      <c r="D100">
+        <v>3.8108999999999997E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>4.5760000000000002E-2</v>
+      </c>
+      <c r="D101">
+        <v>4.6525999999999998E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>4.2813999999999998E-2</v>
+      </c>
+      <c r="D102">
+        <v>4.2851E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>5.9499000000000003E-2</v>
+      </c>
+      <c r="D103">
+        <v>5.9090999999999998E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>4.3457000000000003E-2</v>
+      </c>
+      <c r="D104">
+        <v>4.3318000000000002E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>3.8013999999999999E-2</v>
+      </c>
+      <c r="D105">
+        <v>3.8406999999999997E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>5.4787000000000002E-2</v>
+      </c>
+      <c r="D106">
+        <v>5.4553999999999998E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>5.8714000000000002E-2</v>
+      </c>
+      <c r="D107">
+        <v>5.8442000000000001E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>9.6389000000000002E-2</v>
+      </c>
+      <c r="D108">
+        <v>9.6869999999999998E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>8.4061999999999998E-2</v>
+      </c>
+      <c r="D109">
+        <v>8.3540000000000003E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>4.4666999999999998E-2</v>
+      </c>
+      <c r="D110">
+        <v>4.4408999999999997E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>6.9706000000000004E-2</v>
+      </c>
+      <c r="D111">
+        <v>6.9474999999999995E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>3.6711000000000001E-2</v>
+      </c>
+      <c r="C112" s="2">
+        <f>ABS(B112-$A27)/$A27</f>
+        <v>0.40693053311793209</v>
+      </c>
+      <c r="D112">
+        <v>3.6725000000000001E-2</v>
+      </c>
+      <c r="E112" s="2">
+        <f>ABS(D112-$A27)/$A27</f>
+        <v>0.40670436187399028</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>3.8838999999999999E-2</v>
+      </c>
+      <c r="C113" s="2">
+        <f t="shared" ref="C113:E115" si="7">ABS(B113-$A28)/$A28</f>
+        <v>7.0837320574162643E-2</v>
+      </c>
+      <c r="D113">
+        <v>3.7263999999999999E-2</v>
+      </c>
+      <c r="E113" s="2">
+        <f t="shared" ref="E113:E115" si="8">ABS(D113-$A28)/$A28</f>
+        <v>0.10851674641148322</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>6.3597000000000001E-2</v>
+      </c>
+      <c r="C114" s="2">
+        <f t="shared" si="7"/>
+        <v>0.58992500000000003</v>
+      </c>
+      <c r="D114">
+        <v>6.2385999999999997E-2</v>
+      </c>
+      <c r="E114" s="2">
+        <f t="shared" si="8"/>
+        <v>0.55964999999999987</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>2.5373E-2</v>
+      </c>
+      <c r="C115" s="2">
+        <f t="shared" si="7"/>
+        <v>0.60844135802469135</v>
+      </c>
+      <c r="D115">
+        <v>2.4118000000000001E-2</v>
+      </c>
+      <c r="E115" s="2">
+        <f t="shared" si="8"/>
+        <v>0.62780864197530861</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C116" s="2">
+        <f>AVERAGE(C112:C115)</f>
+        <v>0.41903355292919653</v>
+      </c>
+      <c r="E116" s="2">
+        <f>AVERAGE(E112:E115)</f>
+        <v>0.4256699375651955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add LR and RNN code for May to Aug analysis
</commit_message>
<xml_diff>
--- a/output_Harris_RNN_opt.xlsx
+++ b/output_Harris_RNN_opt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alano\evaptransmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC804E97-FB5E-421B-98D2-80C524932012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23141CF9-A3C8-45B8-8479-AE7490563D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="2610" windowWidth="21600" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_Harris_RNN_opt" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>actual</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>10-200-1, 1e5</t>
+  </si>
+  <si>
+    <t>1-70-1 1e7</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K116"/>
+  <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2805,7 +2808,7 @@
         <v>3.8838999999999999E-2</v>
       </c>
       <c r="C113" s="2">
-        <f t="shared" ref="C113:E115" si="7">ABS(B113-$A28)/$A28</f>
+        <f t="shared" ref="C113:C115" si="7">ABS(B113-$A28)/$A28</f>
         <v>7.0837320574162643E-2</v>
       </c>
       <c r="D113">
@@ -2856,6 +2859,158 @@
       <c r="E116" s="2">
         <f>AVERAGE(E112:E115)</f>
         <v>0.4256699375651955</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>8.5133E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>4.8994000000000003E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>0.141404</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>0.109572</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>5.7875999999999997E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>0.20765</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>6.4782000000000006E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>8.8372000000000006E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1.9244000000000001E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>3.2551999999999998E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>4.4278999999999999E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>5.1378E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>5.6221E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>4.1706E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>5.1472999999999998E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>4.9985000000000002E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>4.8557999999999997E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>5.296E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>2.6405000000000001E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>4.8238000000000003E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>6.7297999999999997E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>-5.3821000000000001E-2</v>
+      </c>
+      <c r="C140" s="2">
+        <f>ABS(B140-$A27)/$A27</f>
+        <v>1.8694830371567044</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>7.3504E-2</v>
+      </c>
+      <c r="C141" s="2">
+        <f t="shared" ref="C141:C143" si="9">ABS(B141-$A28)/$A28</f>
+        <v>0.75846889952153118</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>-1.7589E-2</v>
+      </c>
+      <c r="C142" s="2">
+        <f t="shared" si="9"/>
+        <v>1.4397249999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>-0.13505200000000001</v>
+      </c>
+      <c r="C143" s="2">
+        <f t="shared" si="9"/>
+        <v>3.0841358024691359</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="2">
+        <f>AVERAGE(C140:C143)</f>
+        <v>1.7879531847868431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>